<commit_message>
updated the firmware file
</commit_message>
<xml_diff>
--- a/docs/2025_May_July_Lithuania_fieldwork/equipment preparation/leituva_ARU_sheet.xlsx
+++ b/docs/2025_May_July_Lithuania_fieldwork/equipment preparation/leituva_ARU_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PhD thesis\Ch7_lietuva_sounds\docs\2025_May_July_Lithuania_fieldwork\equipment preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411EBA49-BE65-4440-B23B-542A9046605C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC33084-37A2-4656-8F37-B62D9CC0FB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17055" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-2220" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="55">
   <si>
     <t>flashed</t>
   </si>
@@ -144,16 +144,52 @@
     <t>SongMini_id</t>
   </si>
   <si>
-    <t>checked_SD</t>
-  </si>
-  <si>
     <t>SMA05536</t>
   </si>
   <si>
-    <t>255.08GB</t>
-  </si>
-  <si>
     <t>missing</t>
+  </si>
+  <si>
+    <t>firmware</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>added the configuration</t>
+  </si>
+  <si>
+    <t>set_local_time</t>
+  </si>
+  <si>
+    <t>SMA05568</t>
+  </si>
+  <si>
+    <t>SMA05545</t>
+  </si>
+  <si>
+    <t>SMA05548</t>
+  </si>
+  <si>
+    <t>SMA05535</t>
+  </si>
+  <si>
+    <t>SMA05619</t>
+  </si>
+  <si>
+    <t>SMA05533</t>
+  </si>
+  <si>
+    <t>SMA05573</t>
+  </si>
+  <si>
+    <t>tested outdoor</t>
+  </si>
+  <si>
+    <t>recognizing SD card as write protected - fixed</t>
+  </si>
+  <si>
+    <t>SMA05550</t>
   </si>
 </sst>
 </file>
@@ -477,26 +513,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="3" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -507,16 +544,19 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -526,17 +566,17 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>32</v>
-      </c>
       <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -546,14 +586,14 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -563,14 +603,14 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -580,14 +620,14 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -597,17 +637,17 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -617,17 +657,17 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>37</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -637,14 +677,14 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -654,14 +694,14 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>8</v>
       </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -671,17 +711,17 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>9</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>37</v>
       </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -691,14 +731,14 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -708,14 +748,14 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>11</v>
       </c>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -725,14 +765,14 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>12</v>
       </c>
-      <c r="G13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -742,14 +782,14 @@
       <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>13</v>
       </c>
-      <c r="G14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -759,17 +799,17 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>14</v>
       </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
       <c r="H15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -779,17 +819,17 @@
       <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>15</v>
       </c>
-      <c r="G16" t="s">
-        <v>32</v>
-      </c>
       <c r="H16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -799,14 +839,14 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>16</v>
       </c>
-      <c r="G17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -816,14 +856,14 @@
       <c r="C18" t="s">
         <v>5</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>17</v>
       </c>
-      <c r="G18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -834,7 +874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -844,11 +884,11 @@
       <c r="C20" t="s">
         <v>5</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -859,7 +899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -870,7 +910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -881,7 +921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -892,7 +932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -903,77 +943,116 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="B29">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E38" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>